<commit_message>
Update to evaluation section + fix citations and references
</commit_message>
<xml_diff>
--- a/data/uk-hack-results/UK_hack_result_chart.xlsx
+++ b/data/uk-hack-results/UK_hack_result_chart.xlsx
@@ -4571,8 +4571,8 @@
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
@@ -4928,7 +4928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
       <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>

</xml_diff>